<commit_message>
starting on a few slides
</commit_message>
<xml_diff>
--- a/explore/openCyto/tcell.xlsx
+++ b/explore/openCyto/tcell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="460" windowWidth="28300" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="2720" yWindow="6560" windowWidth="28300" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>